<commit_message>
Cambio de impresora + Estado STDF
</commit_message>
<xml_diff>
--- a/StgoTech/temp_excel_files/temp_excel_file.xlsx
+++ b/StgoTech/temp_excel_files/temp_excel_file.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -112,13 +112,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -226,13 +226,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -524,7 +524,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
@@ -589,7 +589,11 @@
       </c>
       <c r="S1" s="2" t="n"/>
       <c r="T1" s="2" t="n"/>
-      <c r="U1" s="3" t="inlineStr"/>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="V1" s="3" t="n"/>
       <c r="W1" s="3" t="n"/>
       <c r="X1" s="3" t="n"/>
@@ -815,7 +819,7 @@
     <row r="9" ht="12.6" customHeight="1">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>sn</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B9" s="3" t="n"/>
@@ -836,7 +840,11 @@
       <c r="M9" s="3" t="n"/>
       <c r="N9" s="3" t="n"/>
       <c r="O9" s="3" t="n"/>
-      <c r="P9" s="3" t="inlineStr"/>
+      <c r="P9" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="Q9" s="3" t="n"/>
       <c r="R9" s="3" t="n"/>
       <c r="S9" s="3" t="n"/>
@@ -973,9 +981,7 @@
       <c r="N13" s="5" t="n"/>
       <c r="O13" s="5" t="n"/>
       <c r="P13" s="6" t="n"/>
-      <c r="Q13" s="7" t="n">
-        <v>45226</v>
-      </c>
+      <c r="Q13" s="3" t="n"/>
       <c r="R13" s="3" t="n"/>
       <c r="S13" s="3" t="n"/>
       <c r="T13" s="3" t="n"/>
@@ -993,7 +999,7 @@
       <c r="Z13" s="4" t="n"/>
     </row>
     <row r="14" ht="12.6" customHeight="1">
-      <c r="A14" s="8" t="n"/>
+      <c r="A14" s="7" t="n"/>
       <c r="B14" s="2" t="n"/>
       <c r="C14" s="2" t="n"/>
       <c r="D14" s="2" t="n"/>
@@ -1021,34 +1027,34 @@
       <c r="Z14" s="4" t="n"/>
     </row>
     <row r="15" ht="12.6" customHeight="1">
-      <c r="A15" s="9" t="inlineStr">
+      <c r="A15" s="8" t="inlineStr">
         <is>
           <t>Reparado</t>
         </is>
       </c>
-      <c r="B15" s="9" t="n"/>
-      <c r="C15" s="9" t="n"/>
+      <c r="B15" s="8" t="n"/>
+      <c r="C15" s="8" t="n"/>
       <c r="D15" s="3" t="n"/>
-      <c r="E15" s="9" t="inlineStr">
+      <c r="E15" s="8" t="inlineStr">
         <is>
           <t>Testeado</t>
         </is>
       </c>
-      <c r="F15" s="9" t="n"/>
-      <c r="G15" s="9" t="n"/>
+      <c r="F15" s="8" t="n"/>
+      <c r="G15" s="8" t="n"/>
       <c r="H15" s="3" t="n"/>
-      <c r="I15" s="9" t="inlineStr">
+      <c r="I15" s="8" t="inlineStr">
         <is>
           <t>Nuevo</t>
         </is>
       </c>
-      <c r="J15" s="9" t="n"/>
-      <c r="K15" s="9" t="n"/>
+      <c r="J15" s="8" t="n"/>
+      <c r="K15" s="8" t="n"/>
       <c r="L15" s="3" t="n"/>
-      <c r="M15" s="9" t="n"/>
-      <c r="N15" s="9" t="n"/>
-      <c r="O15" s="9" t="n"/>
-      <c r="P15" s="9" t="n"/>
+      <c r="M15" s="8" t="n"/>
+      <c r="N15" s="8" t="n"/>
+      <c r="O15" s="8" t="n"/>
+      <c r="P15" s="8" t="n"/>
       <c r="Q15" s="3" t="inlineStr">
         <is>
           <t>Fecha Recepción</t>
@@ -1104,7 +1110,11 @@
       <c r="E17" s="3" t="n"/>
       <c r="F17" s="3" t="n"/>
       <c r="G17" s="3" t="n"/>
-      <c r="H17" s="3" t="inlineStr"/>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I17" s="3" t="n"/>
       <c r="J17" s="3" t="n"/>
       <c r="K17" s="3" t="n"/>
@@ -1122,7 +1132,7 @@
       <c r="S17" s="3" t="n"/>
       <c r="T17" s="3" t="inlineStr">
         <is>
-          <t>123sad</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U17" s="3" t="n"/>
@@ -1172,7 +1182,11 @@
       <c r="E19" s="3" t="n"/>
       <c r="F19" s="3" t="n"/>
       <c r="G19" s="3" t="n"/>
-      <c r="H19" s="3" t="inlineStr"/>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I19" s="3" t="n"/>
       <c r="J19" s="3" t="n"/>
       <c r="K19" s="3" t="n"/>
@@ -1188,7 +1202,11 @@
       </c>
       <c r="R19" s="3" t="n"/>
       <c r="S19" s="3" t="n"/>
-      <c r="T19" s="3" t="inlineStr"/>
+      <c r="T19" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="U19" s="3" t="n"/>
       <c r="V19" s="3" t="n"/>
       <c r="W19" s="3" t="n"/>
@@ -1236,7 +1254,11 @@
       <c r="E21" s="3" t="n"/>
       <c r="F21" s="3" t="n"/>
       <c r="G21" s="3" t="n"/>
-      <c r="H21" s="3" t="inlineStr"/>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I21" s="3" t="n"/>
       <c r="J21" s="3" t="n"/>
       <c r="K21" s="3" t="n"/>
@@ -1252,7 +1274,11 @@
       </c>
       <c r="R21" s="3" t="n"/>
       <c r="S21" s="3" t="n"/>
-      <c r="T21" s="3" t="inlineStr"/>
+      <c r="T21" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="U21" s="3" t="n"/>
       <c r="V21" s="3" t="n"/>
       <c r="W21" s="3" t="n"/>
@@ -1300,7 +1326,11 @@
       <c r="E23" s="3" t="n"/>
       <c r="F23" s="3" t="n"/>
       <c r="G23" s="3" t="n"/>
-      <c r="H23" s="3" t="inlineStr"/>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I23" s="3" t="n"/>
       <c r="J23" s="3" t="n"/>
       <c r="K23" s="3" t="n"/>
@@ -1360,7 +1390,11 @@
       <c r="E25" s="3" t="n"/>
       <c r="F25" s="3" t="n"/>
       <c r="G25" s="3" t="n"/>
-      <c r="H25" s="3" t="inlineStr"/>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I25" s="3" t="n"/>
       <c r="J25" s="3" t="n"/>
       <c r="K25" s="3" t="n"/>
@@ -1375,7 +1409,7 @@
       <c r="P25" s="3" t="n"/>
       <c r="Q25" s="3" t="n"/>
       <c r="R25" s="3" t="n"/>
-      <c r="S25" s="7" t="n">
+      <c r="S25" s="9" t="n">
         <v>45226</v>
       </c>
       <c r="T25" s="3" t="n"/>
@@ -1517,7 +1551,11 @@
       <c r="T29" s="3" t="n"/>
       <c r="U29" s="3" t="n"/>
       <c r="V29" s="3" t="n"/>
-      <c r="W29" s="3" t="n"/>
+      <c r="W29" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="X29" s="3" t="n"/>
       <c r="Y29" s="3" t="n"/>
       <c r="Z29" s="4" t="n"/>
@@ -1550,7 +1588,11 @@
       <c r="Q30" s="10" t="n"/>
       <c r="R30" s="10" t="n"/>
       <c r="S30" s="10" t="n"/>
-      <c r="T30" s="3" t="n"/>
+      <c r="T30" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="U30" s="3" t="n"/>
       <c r="V30" s="3" t="n"/>
       <c r="W30" s="3" t="n"/>
@@ -1586,7 +1628,11 @@
       <c r="Q31" s="10" t="n"/>
       <c r="R31" s="10" t="n"/>
       <c r="S31" s="10" t="n"/>
-      <c r="T31" s="3" t="n"/>
+      <c r="T31" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="U31" s="3" t="n"/>
       <c r="V31" s="3" t="n"/>
       <c r="W31" s="3" t="n"/>
@@ -1622,7 +1668,11 @@
       <c r="Q32" s="10" t="n"/>
       <c r="R32" s="10" t="n"/>
       <c r="S32" s="10" t="n"/>
-      <c r="T32" s="3" t="n"/>
+      <c r="T32" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="U32" s="3" t="n"/>
       <c r="V32" s="3" t="n"/>
       <c r="W32" s="3" t="n"/>
@@ -1661,7 +1711,11 @@
       <c r="T33" s="3" t="n"/>
       <c r="U33" s="3" t="n"/>
       <c r="V33" s="3" t="n"/>
-      <c r="W33" s="3" t="n"/>
+      <c r="W33" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="X33" s="3" t="n"/>
       <c r="Y33" s="3" t="n"/>
       <c r="Z33" s="4" t="n"/>
@@ -1697,7 +1751,11 @@
       <c r="T34" s="3" t="n"/>
       <c r="U34" s="3" t="n"/>
       <c r="V34" s="3" t="n"/>
-      <c r="W34" s="3" t="n"/>
+      <c r="W34" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="X34" s="3" t="n"/>
       <c r="Y34" s="3" t="n"/>
       <c r="Z34" s="4" t="n"/>
@@ -1733,7 +1791,11 @@
       <c r="T35" s="3" t="n"/>
       <c r="U35" s="3" t="n"/>
       <c r="V35" s="3" t="n"/>
-      <c r="W35" s="3" t="n"/>
+      <c r="W35" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="X35" s="3" t="n"/>
       <c r="Y35" s="3" t="n"/>
       <c r="Z35" s="4" t="n"/>
@@ -1769,7 +1831,11 @@
       <c r="T36" s="3" t="n"/>
       <c r="U36" s="3" t="n"/>
       <c r="V36" s="3" t="n"/>
-      <c r="W36" s="3" t="n"/>
+      <c r="W36" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="X36" s="3" t="n"/>
       <c r="Y36" s="3" t="n"/>
       <c r="Z36" s="4" t="n"/>
@@ -1805,7 +1871,11 @@
       <c r="T37" s="3" t="n"/>
       <c r="U37" s="3" t="n"/>
       <c r="V37" s="3" t="n"/>
-      <c r="W37" s="3" t="n"/>
+      <c r="W37" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="X37" s="3" t="n"/>
       <c r="Y37" s="3" t="n"/>
       <c r="Z37" s="4" t="n"/>
@@ -1838,7 +1908,11 @@
       <c r="Q38" s="10" t="n"/>
       <c r="R38" s="10" t="n"/>
       <c r="S38" s="10" t="n"/>
-      <c r="T38" s="3" t="n"/>
+      <c r="T38" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="U38" s="3" t="n"/>
       <c r="V38" s="3" t="n"/>
       <c r="W38" s="3" t="n"/>
@@ -1874,7 +1948,11 @@
       <c r="Q39" s="10" t="n"/>
       <c r="R39" s="10" t="n"/>
       <c r="S39" s="10" t="n"/>
-      <c r="T39" s="3" t="n"/>
+      <c r="T39" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="U39" s="3" t="n"/>
       <c r="V39" s="3" t="n"/>
       <c r="W39" s="3" t="n"/>
@@ -1910,7 +1988,11 @@
       <c r="Q40" s="10" t="n"/>
       <c r="R40" s="10" t="n"/>
       <c r="S40" s="10" t="n"/>
-      <c r="T40" s="3" t="n"/>
+      <c r="T40" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="U40" s="3" t="n"/>
       <c r="V40" s="3" t="n"/>
       <c r="W40" s="3" t="n"/>
@@ -1946,11 +2028,17 @@
           <t>N°</t>
         </is>
       </c>
-      <c r="P41" s="10" t="n"/>
+      <c r="P41" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="Q41" s="10" t="n"/>
       <c r="R41" s="10" t="n"/>
       <c r="S41" s="10" t="n"/>
-      <c r="T41" s="3" t="n"/>
+      <c r="T41" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="U41" s="3" t="n"/>
       <c r="V41" s="3" t="n"/>
       <c r="W41" s="3" t="n"/>
@@ -2069,7 +2157,11 @@
       <c r="T44" s="3" t="n"/>
       <c r="U44" s="3" t="n"/>
       <c r="V44" s="3" t="n"/>
-      <c r="W44" s="3" t="n"/>
+      <c r="W44" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="X44" s="3" t="n"/>
       <c r="Y44" s="3" t="n"/>
       <c r="Z44" s="4" t="n"/>
@@ -2099,14 +2191,20 @@
           <t>N°</t>
         </is>
       </c>
-      <c r="M45" s="10" t="n"/>
+      <c r="M45" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="N45" s="10" t="n"/>
       <c r="O45" s="10" t="n"/>
       <c r="P45" s="10" t="n"/>
       <c r="Q45" s="10" t="n"/>
       <c r="R45" s="10" t="n"/>
       <c r="S45" s="10" t="n"/>
-      <c r="T45" s="3" t="n"/>
+      <c r="T45" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="U45" s="3" t="n"/>
       <c r="V45" s="3" t="n"/>
       <c r="W45" s="3" t="n"/>
@@ -2377,7 +2475,7 @@
     <row r="53" ht="12.6" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>sn</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B53" s="3" t="n"/>
@@ -2561,7 +2659,7 @@
       <c r="D59" s="3" t="n"/>
       <c r="E59" s="10" t="inlineStr">
         <is>
-          <t>123sad</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F59" s="10" t="n"/>
@@ -2901,7 +2999,11 @@
       <c r="F69" s="3" t="n"/>
       <c r="G69" s="3" t="n"/>
       <c r="H69" s="3" t="n"/>
-      <c r="I69" s="3" t="inlineStr"/>
+      <c r="I69" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="J69" s="3" t="n"/>
       <c r="K69" s="3" t="n"/>
       <c r="L69" s="3" t="n"/>
@@ -3211,6 +3313,6 @@
     <mergeCell ref="M15:P15"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.3" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>